<commit_message>
New Q's and Debrief Screen
Quiz directions and new questions
</commit_message>
<xml_diff>
--- a/pages/upload_select/QuestionBank.xlsx
+++ b/pages/upload_select/QuestionBank.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/traj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/EmployEDU/pages/upload_select/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="2480" yWindow="2560" windowWidth="23680" windowHeight="10740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -510,7 +512,7 @@
         <v>14</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>9</v>
@@ -550,7 +552,7 @@
         <v>14</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
@@ -570,7 +572,7 @@
         <v>22</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>

</xml_diff>